<commit_message>
web app for viewing
</commit_message>
<xml_diff>
--- a/Spring 2026 Sections.xlsx
+++ b/Spring 2026 Sections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/craigbakke/Projects/Python/wit-schedule-maker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D842BE-4A64-3A4A-A07D-B290DD02B8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5783F8C4-60F7-0244-BBAA-68AE2364FC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>Course Title</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t>Sucharita Sen-Banerjee</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>Leonidas Deligiannidis</t>
+  </si>
+  <si>
+    <t>System Administration</t>
+  </si>
+  <si>
+    <t>Security Principles</t>
+  </si>
+  <si>
+    <t>Network Administration</t>
   </si>
 </sst>
 </file>
@@ -628,15 +643,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30:S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
@@ -759,6 +774,9 @@
       <c r="P2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Q2" s="13">
+        <v>4.2</v>
+      </c>
       <c r="R2" s="12" t="b">
         <v>1</v>
       </c>
@@ -815,6 +833,9 @@
       <c r="P3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Q3" s="13">
+        <v>4.2</v>
+      </c>
       <c r="R3" s="12" t="b">
         <v>1</v>
       </c>
@@ -871,6 +892,9 @@
       <c r="P4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Q4" s="13">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="R4" s="12" t="b">
         <v>1</v>
       </c>
@@ -927,8 +951,11 @@
       <c r="P5" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Q5" s="13">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="R5" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="16">
         <v>1</v>
@@ -984,7 +1011,7 @@
         <v>24</v>
       </c>
       <c r="R6" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" s="16">
         <v>1</v>
@@ -1039,6 +1066,9 @@
       <c r="P7" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="Q7" s="13">
+        <v>2.8</v>
+      </c>
       <c r="R7" s="12" t="b">
         <v>1</v>
       </c>
@@ -1095,8 +1125,11 @@
       <c r="P8" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="Q8" s="13">
+        <v>2.8</v>
+      </c>
       <c r="R8" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="16">
         <v>2</v>
@@ -1152,7 +1185,7 @@
         <v>26</v>
       </c>
       <c r="R9" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="16">
         <v>2</v>
@@ -1208,7 +1241,7 @@
         <v>26</v>
       </c>
       <c r="R10" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="16">
         <v>2</v>
@@ -1307,8 +1340,11 @@
       <c r="P12" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="Q12" s="13">
+        <v>2.1</v>
+      </c>
       <c r="R12" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="16">
         <v>3</v>
@@ -1357,8 +1393,11 @@
       <c r="P13" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="Q13" s="13">
+        <v>2.1</v>
+      </c>
       <c r="R13" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="16">
         <v>3</v>
@@ -1407,8 +1446,11 @@
       <c r="P14" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="Q14" s="13">
+        <v>3.4</v>
+      </c>
       <c r="R14" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="16">
         <v>3</v>
@@ -1457,8 +1499,11 @@
       <c r="P15" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="Q15" s="13">
+        <v>3.4</v>
+      </c>
       <c r="R15" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" s="16">
         <v>3</v>
@@ -1507,6 +1552,9 @@
       <c r="P16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="Q16" s="13">
+        <v>5</v>
+      </c>
       <c r="R16" s="12" t="b">
         <v>1</v>
       </c>
@@ -1557,6 +1605,9 @@
       <c r="P17" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="Q17" s="13">
+        <v>3.8</v>
+      </c>
       <c r="R17" s="12" t="b">
         <v>1</v>
       </c>
@@ -1607,6 +1658,9 @@
       <c r="P18" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="Q18" s="13">
+        <v>3.8</v>
+      </c>
       <c r="R18" s="12" t="b">
         <v>1</v>
       </c>
@@ -1663,8 +1717,11 @@
       <c r="P19" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="Q19" s="13">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="R19" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19" s="16">
         <v>4</v>
@@ -1719,8 +1776,11 @@
       <c r="P20" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="Q20" s="13">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="R20" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20" s="16">
         <v>4</v>
@@ -1775,8 +1835,11 @@
       <c r="P21" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="Q21" s="13">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="R21" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" s="16">
         <v>4</v>
@@ -1831,6 +1894,9 @@
       <c r="P22" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="Q22" s="13">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="R22" s="12" t="b">
         <v>1</v>
       </c>
@@ -1887,6 +1953,9 @@
       <c r="P23" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="Q23" s="13">
+        <v>3.9</v>
+      </c>
       <c r="R23" s="12" t="b">
         <v>1</v>
       </c>
@@ -1943,8 +2012,11 @@
       <c r="P24" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="Q24" s="13">
+        <v>3.8</v>
+      </c>
       <c r="R24" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" s="16">
         <v>4</v>
@@ -2111,6 +2183,9 @@
       <c r="P27" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="Q27" s="13">
+        <v>3.8</v>
+      </c>
       <c r="R27" s="12" t="b">
         <v>1</v>
       </c>
@@ -2167,6 +2242,9 @@
       <c r="P28" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="Q28" s="13">
+        <v>3.8</v>
+      </c>
       <c r="R28" s="12" t="b">
         <v>1</v>
       </c>
@@ -2174,8 +2252,547 @@
         <v>4</v>
       </c>
     </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1100</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1215</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>1000</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1145</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" s="13">
+        <v>3.6</v>
+      </c>
+      <c r="R29" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S29" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1230</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1345</v>
+      </c>
+      <c r="I30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1300</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1445</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R30" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7">
+        <v>800</v>
+      </c>
+      <c r="H31" s="8">
+        <v>915</v>
+      </c>
+      <c r="I31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <v>800</v>
+      </c>
+      <c r="O31" s="2">
+        <v>945</v>
+      </c>
+      <c r="R31" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1400</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1515</v>
+      </c>
+      <c r="I32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>1300</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1445</v>
+      </c>
+      <c r="R32" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1530</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1645</v>
+      </c>
+      <c r="I33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>1500</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1645</v>
+      </c>
+      <c r="R33" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S33" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1530</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1645</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3">
+        <v>1500</v>
+      </c>
+      <c r="O34" s="2">
+        <v>1645</v>
+      </c>
+      <c r="R34" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S34" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
+        <v>800</v>
+      </c>
+      <c r="H35" s="8">
+        <v>915</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N35" s="3">
+        <v>800</v>
+      </c>
+      <c r="O35" s="2">
+        <v>945</v>
+      </c>
+      <c r="R35" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S35" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1230</v>
+      </c>
+      <c r="H36" s="8">
+        <v>1345</v>
+      </c>
+      <c r="I36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <v>1300</v>
+      </c>
+      <c r="O36" s="2">
+        <v>1445</v>
+      </c>
+      <c r="R36" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S36" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1530</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1645</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
+        <v>1500</v>
+      </c>
+      <c r="O37" s="2">
+        <v>1645</v>
+      </c>
+      <c r="R37" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S37" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1400</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1515</v>
+      </c>
+      <c r="I38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" s="3">
+        <v>1500</v>
+      </c>
+      <c r="O38" s="2">
+        <v>1645</v>
+      </c>
+      <c r="R38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S38" s="16">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N1:P23 G1:H1048576 N29:P1048576 N24:O28">
+  <conditionalFormatting sqref="N1:P23 N24:O28 G1:H1048576 N29:P1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>